<commit_message>
including articles for testing
</commit_message>
<xml_diff>
--- a/data/evaluation/robin_chatbot_test.xlsx
+++ b/data/evaluation/robin_chatbot_test.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2781,7 +2781,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2861,7 +2861,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3141,7 +3141,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3381,7 +3381,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3621,7 +3621,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3901,7 +3901,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -4121,7 +4121,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
+          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">

</xml_diff>

<commit_message>
model upgrade and changes in file chain
</commit_message>
<xml_diff>
--- a/data/evaluation/robin_chatbot_test.xlsx
+++ b/data/evaluation/robin_chatbot_test.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence concealment and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence concealment.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the allocation sequence randomization and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the allocation sequence randomization.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2781,7 +2781,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2861,7 +2861,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3141,7 +3141,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of outcome assessors and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of outcome assessors.</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3381,7 +3381,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3621,7 +3621,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3901,7 +3901,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -4121,7 +4121,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Use the risk of bias tool to evaluate the risk of bias concerning the blinding of participants, and personnel and provide evidence for supporting it.</t>
+          <t>Evaluate the risk of bias concerning the blinding of participants, and personnel.</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">

</xml_diff>